<commit_message>
Reduced lines of code + data
</commit_message>
<xml_diff>
--- a/Tables/Specific Condenser Duty performance.xlsx
+++ b/Tables/Specific Condenser Duty performance.xlsx
@@ -55,7 +55,7 @@
     <t>SV_ConsSD</t>
   </si>
   <si>
-    <t>DN_ConsSD</t>
+    <t>DL_ConsSD</t>
   </si>
 </sst>
 </file>
@@ -485,25 +485,25 @@
         <v>0.9997757524042872</v>
       </c>
       <c r="C3">
-        <v>0.008564035773174003</v>
+        <v>0.008564035773174005</v>
       </c>
       <c r="D3">
-        <v>0.004427547437360635</v>
+        <v>0.004427547437360639</v>
       </c>
       <c r="E3">
-        <v>0.01634454154301982</v>
+        <v>0.01634454154301983</v>
       </c>
       <c r="F3">
         <v>0.999110040884568</v>
       </c>
       <c r="G3">
-        <v>0.01496273640566522</v>
+        <v>0.01496273640566521</v>
       </c>
       <c r="H3">
         <v>0.006244082824812786</v>
       </c>
       <c r="I3">
-        <v>0.03256071053709743</v>
+        <v>0.03256071053709742</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -569,28 +569,28 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0.9982786846033488</v>
+        <v>0.9982786914031656</v>
       </c>
       <c r="C6">
-        <v>0.03161803710349252</v>
+        <v>0.03161798606353385</v>
       </c>
       <c r="D6">
-        <v>0.01468103118806651</v>
+        <v>0.01468101875194277</v>
       </c>
       <c r="E6">
-        <v>0.04528340468255552</v>
+        <v>0.04528331523957421</v>
       </c>
       <c r="F6">
-        <v>0.9818873546665895</v>
+        <v>0.9818873422160905</v>
       </c>
       <c r="G6">
-        <v>0.112858151889293</v>
+        <v>0.1128581830842473</v>
       </c>
       <c r="H6">
-        <v>0.06060161201380963</v>
+        <v>0.06060163320539391</v>
       </c>
       <c r="I6">
-        <v>0.1468925557952813</v>
+        <v>0.146892606281703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>